<commit_message>
Added some visual changes, project fnished (for now :))
</commit_message>
<xml_diff>
--- a/DaneWojewodztwa2023.xlsx
+++ b/DaneWojewodztwa2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\R tora\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\analiza\Analiza\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8FE72E-A828-48BB-8761-08BCFFD26493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F6C233-AFD4-4C20-8F1B-CA22AF92A3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6570" yWindow="2295" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DaneWojewodztwa2023" sheetId="1" r:id="rId1"/>
@@ -959,7 +959,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>